<commit_message>
Added Sno column with Correct column names
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,306 +397,660 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:AR26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>name</v>
+        <v>SNO</v>
       </c>
       <c r="B1" t="str">
-        <v>companyEmail</v>
+        <v>Unit</v>
       </c>
       <c r="C1" t="str">
-        <v>linkedinUrl</v>
+        <v>Type of Eqpt</v>
       </c>
       <c r="D1" t="str">
-        <v>contactNumber</v>
+        <v>Issue Type</v>
       </c>
       <c r="E1" t="str">
-        <v>yourHRIS</v>
+        <v>BA No</v>
       </c>
       <c r="F1" t="str">
-        <v>unit</v>
+        <v>Chassis No</v>
       </c>
       <c r="G1" t="str">
-        <v>typeOfEquipment</v>
+        <v>Engine Org/OH</v>
       </c>
       <c r="H1" t="str">
-        <v>issueType</v>
+        <v>Eng Km</v>
       </c>
       <c r="I1" t="str">
-        <v>baNo</v>
+        <v>Eng Hrs</v>
       </c>
       <c r="J1" t="str">
-        <v>chassisNo</v>
+        <v>Chassis Km</v>
       </c>
       <c r="K1" t="str">
-        <v>engineOrgOH</v>
+        <v>Chassis Hrs</v>
       </c>
       <c r="L1" t="str">
-        <v>engKm</v>
+        <v>TM I Done</v>
       </c>
       <c r="M1" t="str">
-        <v>engHrs</v>
+        <v>TM I Due</v>
       </c>
       <c r="N1" t="str">
-        <v>chassisKm</v>
+        <v>TM II Done</v>
       </c>
       <c r="O1" t="str">
-        <v>chassisHrs</v>
+        <v>TM II Due</v>
       </c>
       <c r="P1" t="str">
-        <v>tmIDone</v>
+        <v>MR-I Due Dt</v>
       </c>
       <c r="Q1" t="str">
-        <v>tmIDue</v>
+        <v>MR-I Done Dt</v>
       </c>
       <c r="R1" t="str">
-        <v>tmIIDone</v>
+        <v>OH-I Due Dt</v>
       </c>
       <c r="S1" t="str">
-        <v>tmIIDue</v>
+        <v>OH-I Done Dt</v>
       </c>
       <c r="T1" t="str">
-        <v>mrIDueDt</v>
+        <v>MR II Due</v>
       </c>
       <c r="U1" t="str">
-        <v>mrIDoneDt</v>
+        <v>MR II Done</v>
       </c>
       <c r="V1" t="str">
-        <v>ohIDueDt</v>
+        <v>OH II Due</v>
       </c>
       <c r="W1" t="str">
-        <v>ohIDoneDt</v>
+        <v>OH II Done</v>
       </c>
       <c r="X1" t="str">
-        <v>mrIIDue</v>
+        <v>SER/R2/EOA/VOR</v>
       </c>
       <c r="Y1" t="str">
-        <v>mrIIDone</v>
+        <v>Assy</v>
       </c>
       <c r="Z1" t="str">
-        <v>ohIIDue</v>
+        <v>Section</v>
       </c>
       <c r="AA1" t="str">
-        <v>ohIIDone</v>
+        <v>Nature of Defect</v>
       </c>
       <c r="AB1" t="str">
-        <v>serR2EOAVOR</v>
+        <v>Demand Placed To</v>
       </c>
       <c r="AC1" t="str">
-        <v>assy</v>
+        <v>Demand No &amp; Dt</v>
       </c>
       <c r="AD1" t="str">
-        <v>section</v>
+        <v>Cont No &amp; Dt</v>
       </c>
       <c r="AE1" t="str">
-        <v>natureOfDefect</v>
+        <v>Work Order No &amp; Dt</v>
       </c>
       <c r="AF1" t="str">
-        <v>demandPlacedTo</v>
+        <v>Fwd To</v>
       </c>
       <c r="AG1" t="str">
-        <v>demandNoDt</v>
+        <v>Since</v>
       </c>
       <c r="AH1" t="str">
-        <v>contNoDt</v>
+        <v>Present Status</v>
       </c>
       <c r="AI1" t="str">
-        <v>workOrderNoDate</v>
+        <v>Under Repair Time</v>
       </c>
       <c r="AJ1" t="str">
-        <v>fwdTo</v>
+        <v>EFC/RDS Fired</v>
       </c>
       <c r="AK1" t="str">
-        <v>since</v>
+        <v>Chamber Elongation</v>
       </c>
       <c r="AL1" t="str">
-        <v>presentStatus</v>
+        <v>Bore</v>
       </c>
       <c r="AM1" t="str">
-        <v>underRepairTime</v>
+        <v>Gun Pull Back Done Date</v>
       </c>
       <c r="AN1" t="str">
-        <v>efcRDSFired</v>
+        <v>SI Details</v>
       </c>
       <c r="AO1" t="str">
-        <v>chamberElongation</v>
+        <v>Fume Extractor</v>
       </c>
       <c r="AP1" t="str">
-        <v>bore</v>
+        <v>N2 Purging Due Date</v>
       </c>
       <c r="AQ1" t="str">
-        <v>gunPullBackDoneDate</v>
+        <v>N2 Purging Carried Out</v>
       </c>
       <c r="AR1" t="str">
-        <v>siDetails</v>
-      </c>
-      <c r="AS1" t="str">
-        <v>fumeExtractor</v>
-      </c>
-      <c r="AT1" t="str">
-        <v>n2PurgingDueDate</v>
-      </c>
-      <c r="AU1" t="str">
-        <v>n2PurgingCarriedOut</v>
-      </c>
-      <c r="AV1" t="str">
-        <v>getterActivationDoneDate</v>
+        <v>Getter Activation Done Date (Check Every 3 Months)</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v/>
-      </c>
-      <c r="B2" t="str">
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="M2" t="str">
-        <v/>
-      </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
-      <c r="O2" t="str">
-        <v/>
-      </c>
-      <c r="P2" t="str">
-        <v/>
-      </c>
-      <c r="Q2" t="str">
-        <v/>
-      </c>
-      <c r="R2" t="str">
-        <v/>
-      </c>
-      <c r="S2" t="str">
-        <v/>
-      </c>
-      <c r="T2" t="str">
-        <v/>
-      </c>
-      <c r="U2" t="str">
-        <v/>
-      </c>
-      <c r="V2" t="str">
-        <v/>
-      </c>
-      <c r="W2" t="str">
-        <v/>
-      </c>
-      <c r="X2" t="str">
-        <v/>
-      </c>
-      <c r="Y2" t="str">
-        <v/>
-      </c>
-      <c r="Z2" t="str">
-        <v/>
-      </c>
-      <c r="AA2" t="str">
-        <v/>
-      </c>
-      <c r="AB2" t="str">
-        <v/>
-      </c>
-      <c r="AC2" t="str">
-        <v/>
-      </c>
-      <c r="AD2" t="str">
-        <v/>
-      </c>
-      <c r="AE2" t="str">
-        <v/>
-      </c>
-      <c r="AF2" t="str">
-        <v/>
-      </c>
-      <c r="AG2" t="str">
-        <v/>
-      </c>
-      <c r="AH2" t="str">
-        <v/>
-      </c>
-      <c r="AI2" t="str">
-        <v/>
-      </c>
-      <c r="AJ2" t="str">
-        <v/>
-      </c>
-      <c r="AK2" t="str">
-        <v/>
-      </c>
-      <c r="AL2" t="str">
-        <v/>
-      </c>
-      <c r="AM2" t="str">
-        <v/>
-      </c>
-      <c r="AN2" t="str">
-        <v/>
-      </c>
-      <c r="AO2" t="str">
-        <v/>
-      </c>
-      <c r="AP2" t="str">
-        <v/>
-      </c>
-      <c r="AQ2" t="str">
-        <v/>
-      </c>
-      <c r="AR2" t="str">
-        <v/>
-      </c>
-      <c r="AS2" t="str">
-        <v/>
-      </c>
-      <c r="AT2" t="str">
-        <v/>
-      </c>
-      <c r="AU2" t="str">
-        <v/>
-      </c>
-      <c r="AV2" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>23</v>
+      </c>
+      <c r="B24" t="str">
+        <v>First</v>
+      </c>
+      <c r="C24" t="str">
+        <v/>
+      </c>
+      <c r="D24" t="str">
+        <v/>
+      </c>
+      <c r="E24" t="str">
+        <v/>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+      <c r="G24" t="str">
+        <v/>
+      </c>
+      <c r="H24" t="str">
+        <v/>
+      </c>
+      <c r="I24" t="str">
+        <v/>
+      </c>
+      <c r="J24" t="str">
+        <v/>
+      </c>
+      <c r="K24" t="str">
+        <v/>
+      </c>
+      <c r="L24" t="str">
+        <v/>
+      </c>
+      <c r="M24" t="str">
+        <v/>
+      </c>
+      <c r="N24" t="str">
+        <v/>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v/>
+      </c>
+      <c r="Q24" t="str">
+        <v/>
+      </c>
+      <c r="R24" t="str">
+        <v/>
+      </c>
+      <c r="S24" t="str">
+        <v/>
+      </c>
+      <c r="T24" t="str">
+        <v/>
+      </c>
+      <c r="U24" t="str">
+        <v/>
+      </c>
+      <c r="V24" t="str">
+        <v/>
+      </c>
+      <c r="W24" t="str">
+        <v/>
+      </c>
+      <c r="X24" t="str">
+        <v/>
+      </c>
+      <c r="Y24" t="str">
+        <v/>
+      </c>
+      <c r="Z24" t="str">
+        <v/>
+      </c>
+      <c r="AA24" t="str">
+        <v/>
+      </c>
+      <c r="AB24" t="str">
+        <v/>
+      </c>
+      <c r="AC24" t="str">
+        <v/>
+      </c>
+      <c r="AD24" t="str">
+        <v/>
+      </c>
+      <c r="AE24" t="str">
+        <v/>
+      </c>
+      <c r="AF24" t="str">
+        <v/>
+      </c>
+      <c r="AG24" t="str">
+        <v/>
+      </c>
+      <c r="AH24" t="str">
+        <v/>
+      </c>
+      <c r="AI24" t="str">
+        <v/>
+      </c>
+      <c r="AJ24" t="str">
+        <v/>
+      </c>
+      <c r="AK24" t="str">
+        <v/>
+      </c>
+      <c r="AL24" t="str">
+        <v/>
+      </c>
+      <c r="AM24" t="str">
+        <v/>
+      </c>
+      <c r="AN24" t="str">
+        <v/>
+      </c>
+      <c r="AO24" t="str">
+        <v/>
+      </c>
+      <c r="AP24" t="str">
+        <v/>
+      </c>
+      <c r="AQ24" t="str">
+        <v/>
+      </c>
+      <c r="AR24" t="str">
+        <v>Last</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>24</v>
+      </c>
+      <c r="B25" t="str">
+        <v>First First</v>
+      </c>
+      <c r="C25" t="str">
+        <v/>
+      </c>
+      <c r="D25" t="str">
+        <v/>
+      </c>
+      <c r="E25" t="str">
+        <v/>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+      <c r="G25" t="str">
+        <v/>
+      </c>
+      <c r="H25" t="str">
+        <v/>
+      </c>
+      <c r="I25" t="str">
+        <v/>
+      </c>
+      <c r="J25" t="str">
+        <v/>
+      </c>
+      <c r="K25" t="str">
+        <v/>
+      </c>
+      <c r="L25" t="str">
+        <v/>
+      </c>
+      <c r="M25" t="str">
+        <v/>
+      </c>
+      <c r="N25" t="str">
+        <v/>
+      </c>
+      <c r="O25" t="str">
+        <v/>
+      </c>
+      <c r="P25" t="str">
+        <v/>
+      </c>
+      <c r="Q25" t="str">
+        <v/>
+      </c>
+      <c r="R25" t="str">
+        <v/>
+      </c>
+      <c r="S25" t="str">
+        <v/>
+      </c>
+      <c r="T25" t="str">
+        <v/>
+      </c>
+      <c r="U25" t="str">
+        <v/>
+      </c>
+      <c r="V25" t="str">
+        <v/>
+      </c>
+      <c r="W25" t="str">
+        <v/>
+      </c>
+      <c r="X25" t="str">
+        <v/>
+      </c>
+      <c r="Y25" t="str">
+        <v/>
+      </c>
+      <c r="Z25" t="str">
+        <v/>
+      </c>
+      <c r="AA25" t="str">
+        <v/>
+      </c>
+      <c r="AB25" t="str">
+        <v/>
+      </c>
+      <c r="AC25" t="str">
+        <v/>
+      </c>
+      <c r="AD25" t="str">
+        <v/>
+      </c>
+      <c r="AE25" t="str">
+        <v/>
+      </c>
+      <c r="AF25" t="str">
+        <v/>
+      </c>
+      <c r="AG25" t="str">
+        <v/>
+      </c>
+      <c r="AH25" t="str">
+        <v/>
+      </c>
+      <c r="AI25" t="str">
+        <v/>
+      </c>
+      <c r="AJ25" t="str">
+        <v/>
+      </c>
+      <c r="AK25" t="str">
+        <v/>
+      </c>
+      <c r="AL25" t="str">
+        <v/>
+      </c>
+      <c r="AM25" t="str">
+        <v/>
+      </c>
+      <c r="AN25" t="str">
+        <v/>
+      </c>
+      <c r="AO25" t="str">
+        <v/>
+      </c>
+      <c r="AP25" t="str">
+        <v/>
+      </c>
+      <c r="AQ25" t="str">
+        <v/>
+      </c>
+      <c r="AR25" t="str">
+        <v>Last Last</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>25</v>
+      </c>
+      <c r="B26" t="str">
+        <v>First First</v>
+      </c>
+      <c r="C26" t="str">
+        <v/>
+      </c>
+      <c r="D26" t="str">
+        <v/>
+      </c>
+      <c r="E26" t="str">
+        <v/>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+      <c r="G26" t="str">
+        <v/>
+      </c>
+      <c r="H26" t="str">
+        <v/>
+      </c>
+      <c r="I26" t="str">
+        <v/>
+      </c>
+      <c r="J26" t="str">
+        <v/>
+      </c>
+      <c r="K26" t="str">
+        <v/>
+      </c>
+      <c r="L26" t="str">
+        <v/>
+      </c>
+      <c r="M26" t="str">
+        <v/>
+      </c>
+      <c r="N26" t="str">
+        <v/>
+      </c>
+      <c r="O26" t="str">
+        <v/>
+      </c>
+      <c r="P26" t="str">
+        <v/>
+      </c>
+      <c r="Q26" t="str">
+        <v/>
+      </c>
+      <c r="R26" t="str">
+        <v/>
+      </c>
+      <c r="S26" t="str">
+        <v/>
+      </c>
+      <c r="T26" t="str">
+        <v/>
+      </c>
+      <c r="U26" t="str">
+        <v/>
+      </c>
+      <c r="V26" t="str">
+        <v/>
+      </c>
+      <c r="W26" t="str">
+        <v/>
+      </c>
+      <c r="X26" t="str">
+        <v/>
+      </c>
+      <c r="Y26" t="str">
+        <v/>
+      </c>
+      <c r="Z26" t="str">
+        <v/>
+      </c>
+      <c r="AA26" t="str">
+        <v/>
+      </c>
+      <c r="AB26" t="str">
+        <v/>
+      </c>
+      <c r="AC26" t="str">
+        <v/>
+      </c>
+      <c r="AD26" t="str">
+        <v/>
+      </c>
+      <c r="AE26" t="str">
+        <v/>
+      </c>
+      <c r="AF26" t="str">
+        <v/>
+      </c>
+      <c r="AG26" t="str">
+        <v/>
+      </c>
+      <c r="AH26" t="str">
+        <v/>
+      </c>
+      <c r="AI26" t="str">
+        <v/>
+      </c>
+      <c r="AJ26" t="str">
+        <v/>
+      </c>
+      <c r="AK26" t="str">
+        <v/>
+      </c>
+      <c r="AL26" t="str">
+        <v/>
+      </c>
+      <c r="AM26" t="str">
+        <v/>
+      </c>
+      <c r="AN26" t="str">
+        <v/>
+      </c>
+      <c r="AO26" t="str">
+        <v/>
+      </c>
+      <c r="AP26" t="str">
+        <v/>
+      </c>
+      <c r="AQ26" t="str">
+        <v/>
+      </c>
+      <c r="AR26" t="str">
+        <v>Last Last</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AV2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AR26"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>